<commit_message>
[save_summary_table] Adding a renaming option for variable names
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -17,7 +17,7 @@
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study.Extracted on : 2022/09/26 11:29:22</t>
+    <t>This is an interesting study.Extracted on : 2022/09/26 11:58:55</t>
   </si>
   <si>
     <t>label</t>
@@ -47,7 +47,7 @@
     <t>texture</t>
   </si>
   <si>
-    <t>compactness_quartile</t>
+    <t>Compactness quartile</t>
   </si>
   <si>
     <t/>
@@ -104,52 +104,52 @@
     <t>116 (54.7)</t>
   </si>
   <si>
-    <t>2.81 (2.37-3.42, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>1.26 (1.2-1.33, p&lt;0.001)</t>
+    <t>2.811 (2.372-3.42, p=1e-28)</t>
+  </si>
+  <si>
+    <t>1.264 (1.203-1.333, p=3e-19)</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>2.71 (1.24-6.42, p=0.016)</t>
-  </si>
-  <si>
-    <t>12.47 (6.16-28.14, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>65.93 (31.13-155.48, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>4.04 (3.07-5.64, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>1.33 (1.26-1.41, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>3.4 (1.4-8.97, p=0.0093)</t>
-  </si>
-  <si>
-    <t>12.69 (5.42-32.87, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>54.21 (20.66-157.56, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>2.72 (2.2-3.46, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>1.25 (1.16-1.34, p&lt;0.001)</t>
-  </si>
-  <si>
-    <t>0.77 (0.31-1.96, p=0.57)</t>
-  </si>
-  <si>
-    <t>0.52 (0.18-1.52, p=0.23)</t>
-  </si>
-  <si>
-    <t>0.22 (0.05-0.91, p=0.038)</t>
+    <t>2.709 (1.237-6.416, p=0.02)</t>
+  </si>
+  <si>
+    <t>12.475 (6.162-28.139, p=5e-11)</t>
+  </si>
+  <si>
+    <t>65.932 (31.127-155.485, p=8e-25)</t>
+  </si>
+  <si>
+    <t>4.043 (3.073-5.638, p=1e-19)</t>
+  </si>
+  <si>
+    <t>1.331 (1.258-1.414, p=7e-22)</t>
+  </si>
+  <si>
+    <t>3.4 (1.396-8.974, p=0.009)</t>
+  </si>
+  <si>
+    <t>12.686 (5.422-32.866, p=3e-08)</t>
+  </si>
+  <si>
+    <t>54.214 (20.658-157.555, p=1e-14)</t>
+  </si>
+  <si>
+    <t>2.716 (2.204-3.46, p=3e-18)</t>
+  </si>
+  <si>
+    <t>1.246 (1.162-1.341, p=1e-09)</t>
+  </si>
+  <si>
+    <t>0.767 (0.314-1.964, p=0.6)</t>
+  </si>
+  <si>
+    <t>0.524 (0.184-1.516, p=0.2)</t>
+  </si>
+  <si>
+    <t>0.219 (0.051-0.908, p=0.04)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
[save_summary_table] Adding an option for column renaming
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -12,18 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study.Extracted on : 2022/09/26 11:58:55</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>levels</t>
+    <t>This is an interesting study.Extracted on : 2022/09/26 12:12:12</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>B</t>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Compactness quartile</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Mean (SD)</t>
@@ -312,22 +309,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s" s="13">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s" s="13">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s" s="13">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s" s="13">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" ht="30.0" customHeight="true">
@@ -335,22 +332,22 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s" s="13">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s" s="13">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s" s="13">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="30.0" customHeight="true">
@@ -358,91 +355,91 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s" s="13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s" s="13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s" s="13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s" s="13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s" s="13">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" ht="30.0" customHeight="true">
       <c r="A8" t="s" s="7">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s" s="13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s" s="13">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" ht="30.0" customHeight="true">
       <c r="A9" t="s" s="7">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s" s="13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s" s="13">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s" s="13">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s" s="13">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" ht="30.0" customHeight="true">
       <c r="A10" t="s" s="7">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s" s="13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s" s="13">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s" s="13">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s" s="13">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s" s="13">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[save_summary_table] Adding a style for column 2
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -17,7 +17,7 @@
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study.Extracted on : 2022/09/26 12:12:12</t>
+    <t>This is an interesting study. Saved on : 2022/09/26 12:28:58</t>
   </si>
   <si>
     <t>Variables</t>
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -249,6 +249,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -308,7 +312,7 @@
       <c r="A5" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="15">
         <v>12</v>
       </c>
       <c r="C5" t="s" s="13">
@@ -331,7 +335,7 @@
       <c r="A6" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="15">
         <v>12</v>
       </c>
       <c r="C6" t="s" s="13">
@@ -354,7 +358,7 @@
       <c r="A7" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="15">
         <v>13</v>
       </c>
       <c r="C7" t="s" s="13">
@@ -377,7 +381,7 @@
       <c r="A8" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="15">
         <v>14</v>
       </c>
       <c r="C8" t="s" s="13">
@@ -400,7 +404,7 @@
       <c r="A9" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="15">
         <v>15</v>
       </c>
       <c r="C9" t="s" s="13">
@@ -423,7 +427,7 @@
       <c r="A10" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="15">
         <v>16</v>
       </c>
       <c r="C10" t="s" s="13">

</xml_diff>

<commit_message>
[save_summary_table] Adding a function to highlight significant pvalues
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -17,7 +17,7 @@
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study. Saved on : 2022/09/26 12:28:58</t>
+    <t>This is an interesting study. Saved on : 2022/09/26 17:01:55</t>
   </si>
   <si>
     <t>Variables</t>
@@ -185,12 +185,29 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="ADD8E6"/>
+        <bgColor rgb="E6E6FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ADD8E6"/>
+        <bgColor rgb="E6E6FA"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -227,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -252,6 +269,97 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -321,13 +429,13 @@
       <c r="D5" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" t="s" s="18">
         <v>29</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" t="s" s="33">
         <v>35</v>
       </c>
-      <c r="G5" t="s" s="13">
+      <c r="G5" t="s" s="48">
         <v>40</v>
       </c>
     </row>
@@ -344,13 +452,13 @@
       <c r="D6" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="E6" t="s" s="13">
+      <c r="E6" t="s" s="21">
         <v>30</v>
       </c>
-      <c r="F6" t="s" s="13">
+      <c r="F6" t="s" s="36">
         <v>36</v>
       </c>
-      <c r="G6" t="s" s="13">
+      <c r="G6" t="s" s="51">
         <v>41</v>
       </c>
     </row>
@@ -390,10 +498,10 @@
       <c r="D8" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="E8" t="s" s="13">
+      <c r="E8" t="s" s="24">
         <v>32</v>
       </c>
-      <c r="F8" t="s" s="13">
+      <c r="F8" t="s" s="39">
         <v>37</v>
       </c>
       <c r="G8" t="s" s="13">
@@ -413,10 +521,10 @@
       <c r="D9" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="E9" t="s" s="13">
+      <c r="E9" t="s" s="27">
         <v>33</v>
       </c>
-      <c r="F9" t="s" s="13">
+      <c r="F9" t="s" s="42">
         <v>38</v>
       </c>
       <c r="G9" t="s" s="13">
@@ -436,13 +544,13 @@
       <c r="D10" t="s" s="13">
         <v>28</v>
       </c>
-      <c r="E10" t="s" s="13">
+      <c r="E10" t="s" s="30">
         <v>34</v>
       </c>
-      <c r="F10" t="s" s="13">
+      <c r="F10" t="s" s="45">
         <v>39</v>
       </c>
-      <c r="G10" t="s" s="13">
+      <c r="G10" t="s" s="54">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[save_summary_table] Finalizing new function to create custom cell style
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -17,7 +17,7 @@
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study. Saved on : 2022/09/26 17:01:55</t>
+    <t>This is an interesting study. Saved on : 2022/09/26 18:58:54</t>
   </si>
   <si>
     <t>Variables</t>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -256,20 +256,36 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -394,25 +410,25 @@
       </c>
     </row>
     <row r="4" ht="30.0" customHeight="true">
-      <c r="A4" t="s" s="11">
+      <c r="A4" t="s" s="23">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" t="s" s="23">
         <v>3</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" t="s" s="23">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="23">
         <v>5</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" t="s" s="23">
         <v>6</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" t="s" s="23">
         <v>7</v>
       </c>
-      <c r="G4" t="s" s="11">
+      <c r="G4" t="s" s="23">
         <v>8</v>
       </c>
     </row>
@@ -420,22 +436,22 @@
       <c r="A5" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" t="s" s="11">
         <v>17</v>
       </c>
       <c r="D5" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="E5" t="s" s="18">
+      <c r="E5" t="s" s="26">
         <v>29</v>
       </c>
-      <c r="F5" t="s" s="33">
+      <c r="F5" t="s" s="41">
         <v>35</v>
       </c>
-      <c r="G5" t="s" s="48">
+      <c r="G5" t="s" s="56">
         <v>40</v>
       </c>
     </row>
@@ -443,22 +459,22 @@
       <c r="A6" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B6" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="13">
+      <c r="C6" t="s" s="11">
         <v>18</v>
       </c>
       <c r="D6" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="E6" t="s" s="21">
+      <c r="E6" t="s" s="29">
         <v>30</v>
       </c>
-      <c r="F6" t="s" s="36">
+      <c r="F6" t="s" s="44">
         <v>36</v>
       </c>
-      <c r="G6" t="s" s="51">
+      <c r="G6" t="s" s="59">
         <v>41</v>
       </c>
     </row>
@@ -466,22 +482,22 @@
       <c r="A7" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="15">
+      <c r="B7" t="s" s="9">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" t="s" s="11">
         <v>19</v>
       </c>
       <c r="D7" t="s" s="13">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="13">
+      <c r="E7" t="s" s="15">
         <v>31</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" t="s" s="17">
         <v>31</v>
       </c>
-      <c r="G7" t="s" s="13">
+      <c r="G7" t="s" s="19">
         <v>31</v>
       </c>
     </row>
@@ -489,22 +505,22 @@
       <c r="A8" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B8" t="s" s="15">
+      <c r="B8" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="C8" t="s" s="13">
+      <c r="C8" t="s" s="11">
         <v>20</v>
       </c>
       <c r="D8" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="E8" t="s" s="24">
+      <c r="E8" t="s" s="32">
         <v>32</v>
       </c>
-      <c r="F8" t="s" s="39">
+      <c r="F8" t="s" s="47">
         <v>37</v>
       </c>
-      <c r="G8" t="s" s="13">
+      <c r="G8" t="s" s="19">
         <v>42</v>
       </c>
     </row>
@@ -512,22 +528,22 @@
       <c r="A9" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B9" t="s" s="15">
+      <c r="B9" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" t="s" s="11">
         <v>21</v>
       </c>
       <c r="D9" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="E9" t="s" s="27">
+      <c r="E9" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="F9" t="s" s="42">
+      <c r="F9" t="s" s="50">
         <v>38</v>
       </c>
-      <c r="G9" t="s" s="13">
+      <c r="G9" t="s" s="19">
         <v>43</v>
       </c>
     </row>
@@ -535,22 +551,22 @@
       <c r="A10" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="15">
+      <c r="B10" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="C10" t="s" s="13">
+      <c r="C10" t="s" s="11">
         <v>22</v>
       </c>
       <c r="D10" t="s" s="13">
         <v>28</v>
       </c>
-      <c r="E10" t="s" s="30">
+      <c r="E10" t="s" s="38">
         <v>34</v>
       </c>
-      <c r="F10" t="s" s="45">
+      <c r="F10" t="s" s="53">
         <v>39</v>
       </c>
-      <c r="G10" t="s" s="54">
+      <c r="G10" t="s" s="62">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcting bugs for devtools check
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -17,7 +17,7 @@
     <t>Regression logistic study</t>
   </si>
   <si>
-    <t>This is an interesting study. Saved on : 2022/09/27 17:18:39</t>
+    <t>This is an interesting study. Saved on : 2022/09/28 17:56:24</t>
   </si>
   <si>
     <t>Variables</t>
@@ -101,10 +101,10 @@
     <t>116 (54.7)</t>
   </si>
   <si>
-    <t>2.811 (2.372-3.42, p=1e-28)</t>
-  </si>
-  <si>
-    <t>1.264 (1.203-1.333, p=3e-19)</t>
+    <t>2.811 (2.372-3.42, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>1.264 (1.203-1.333, p&lt;0.001)</t>
   </si>
   <si>
     <t>-</t>
@@ -113,31 +113,31 @@
     <t>2.709 (1.237-6.416, p=0.02)</t>
   </si>
   <si>
-    <t>12.475 (6.162-28.139, p=5e-11)</t>
-  </si>
-  <si>
-    <t>65.932 (31.127-155.485, p=8e-25)</t>
-  </si>
-  <si>
-    <t>4.043 (3.073-5.638, p=1e-19)</t>
-  </si>
-  <si>
-    <t>1.331 (1.258-1.414, p=7e-22)</t>
+    <t>12.475 (6.162-28.139, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>65.932 (31.127-155.485, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>4.043 (3.073-5.638, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>1.331 (1.258-1.414, p&lt;0.001)</t>
   </si>
   <si>
     <t>3.4 (1.396-8.974, p=0.009)</t>
   </si>
   <si>
-    <t>12.686 (5.422-32.866, p=3e-08)</t>
-  </si>
-  <si>
-    <t>54.214 (20.658-157.555, p=1e-14)</t>
-  </si>
-  <si>
-    <t>2.716 (2.204-3.46, p=3e-18)</t>
-  </si>
-  <si>
-    <t>1.246 (1.162-1.341, p=1e-09)</t>
+    <t>12.686 (5.422-32.866, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>54.214 (20.658-157.555, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>2.716 (2.204-3.46, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>1.246 (1.162-1.341, p&lt;0.001)</t>
   </si>
   <si>
     <t>0.767 (0.314-1.964, p=0.6)</t>
@@ -289,94 +289,94 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>

</xml_diff>